<commit_message>
feature selection by different iterations
</commit_message>
<xml_diff>
--- a/LogisticRegression/report.xlsx
+++ b/LogisticRegression/report.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harel\Documents\GitRepos\LogisticRegression\LogisticRegression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ella\Documents\Visual Studio 2017\Projects\LogisticRegression\LogisticRegression\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="output" sheetId="1" r:id="rId1"/>
+    <sheet name="Logistic regrssion" sheetId="1" r:id="rId1"/>
+    <sheet name="Feature selection" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>alpha</t>
   </si>
@@ -32,12 +33,24 @@
   <si>
     <t>הראל ולך</t>
   </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>selected feature</t>
+  </si>
+  <si>
+    <t>alpha = 1.5</t>
+  </si>
+  <si>
+    <t>alpha = 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +203,16 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +392,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -532,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,52 +567,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="הדגשה1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="הדגשה2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="הדגשה3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="הדגשה4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="הדגשה5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="הדגשה6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="הערה" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="חישוב" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="טוב" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="טקסט אזהרה" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="טקסט הסברי" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="כותרת" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="כותרת 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="כותרת 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="כותרת 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="כותרת 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="ניטראלי" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="סה&quot;כ" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="פלט" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="קלט" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="רע" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="תא מסומן" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="תא מקושר" xfId="12" builtinId="24" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -603,9 +666,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="he-IL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -696,7 +759,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$13</c:f>
+              <c:f>'Logistic regrssion'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -725,7 +788,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -2234,7 +2297,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$2:$SI$2</c:f>
+              <c:f>'Logistic regrssion'!$A$2:$SI$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -3742,7 +3805,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -3753,7 +3816,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$14</c:f>
+              <c:f>'Logistic regrssion'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3782,7 +3845,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -5291,7 +5354,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$3:$SI$3</c:f>
+              <c:f>'Logistic regrssion'!$A$3:$SI$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -6799,7 +6862,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -6810,7 +6873,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$15</c:f>
+              <c:f>'Logistic regrssion'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6839,7 +6902,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -8348,7 +8411,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$4:$SI$4</c:f>
+              <c:f>'Logistic regrssion'!$A$4:$SI$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -9856,7 +9919,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -9867,7 +9930,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$16</c:f>
+              <c:f>'Logistic regrssion'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9896,7 +9959,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -11405,7 +11468,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$5:$SI$5</c:f>
+              <c:f>'Logistic regrssion'!$A$5:$SI$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -12913,7 +12976,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -12924,7 +12987,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$17</c:f>
+              <c:f>'Logistic regrssion'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12953,7 +13016,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -14462,7 +14525,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$6:$SI$6</c:f>
+              <c:f>'Logistic regrssion'!$A$6:$SI$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -15970,7 +16033,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -15981,7 +16044,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$18</c:f>
+              <c:f>'Logistic regrssion'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -16010,7 +16073,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -17519,7 +17582,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$7:$SI$7</c:f>
+              <c:f>'Logistic regrssion'!$A$7:$SI$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -19027,7 +19090,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -19038,7 +19101,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$A$19</c:f>
+              <c:f>'Logistic regrssion'!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -19069,7 +19132,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$1:$SI$1</c:f>
+              <c:f>'Logistic regrssion'!$A$1:$SI$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -20578,7 +20641,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$A$8:$SI$8</c:f>
+              <c:f>'Logistic regrssion'!$A$8:$SI$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="503"/>
@@ -22086,7 +22149,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-6638-47AD-B280-E22015E6BC20}"/>
             </c:ext>
@@ -22101,11 +22164,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="927881280"/>
-        <c:axId val="927871488"/>
+        <c:axId val="-57554960"/>
+        <c:axId val="-57541904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="927881280"/>
+        <c:axId val="-57554960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22147,7 +22210,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="927871488"/>
+        <c:crossAx val="-57541904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22155,7 +22218,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="927871488"/>
+        <c:axId val="-57541904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22205,7 +22268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="927881280"/>
+        <c:crossAx val="-57554960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22297,9 +22360,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="he-IL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -22397,7 +22460,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$B$12</c:f>
+              <c:f>'Logistic regrssion'!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -22468,7 +22531,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$13:$A$19</c:f>
+              <c:f>'Logistic regrssion'!$A$13:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -22498,7 +22561,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$B$13:$B$19</c:f>
+              <c:f>'Logistic regrssion'!$B$13:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -22527,7 +22590,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B47C-4DA8-A05B-0FAE54CE8FA1}"/>
             </c:ext>
@@ -22538,7 +22601,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>output!$C$12</c:f>
+              <c:f>'Logistic regrssion'!$C$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -22609,7 +22672,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>output!$A$13:$A$19</c:f>
+              <c:f>'Logistic regrssion'!$A$13:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -22639,7 +22702,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>output!$C$13:$C$19</c:f>
+              <c:f>'Logistic regrssion'!$C$13:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -22668,7 +22731,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B47C-4DA8-A05B-0FAE54CE8FA1}"/>
             </c:ext>
@@ -22684,11 +22747,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="927869312"/>
-        <c:axId val="927872576"/>
+        <c:axId val="-57544624"/>
+        <c:axId val="-57544080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="927869312"/>
+        <c:axId val="-57544624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22730,7 +22793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="927872576"/>
+        <c:crossAx val="-57544080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -22738,7 +22801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="927872576"/>
+        <c:axId val="-57544080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22788,7 +22851,1146 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="927869312"/>
+        <c:crossAx val="-57544624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>alpha=1.5</a:t>
+            </a:r>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature selection'!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction on test data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature selection'!$N$4:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature selection'!$O$4:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.39405200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95167299999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94795499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94423800000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94423800000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature selection'!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction on training data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature selection'!$N$4:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature selection'!$P$4:$P$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.60333300000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.906667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93333299999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1947593024"/>
+        <c:axId val="-1947590848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1947593024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1947590848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1947590848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>prediction</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1947593024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="he-IL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>alpha=2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.43297922134733158"/>
+          <c:y val="4.6296296296296294E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature selection'!$O$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction on test data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature selection'!$N$26:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature selection'!$O$26:$O$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.44609700000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94052000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94423800000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94423800000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97397800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature selection'!$P$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>prediction on training data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature selection'!$N$26:$N$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature selection'!$P$26:$P$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.62333300000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2041810208"/>
+        <c:axId val="-2051030976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2041810208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="he-IL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2051030976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2051030976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>predictions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2041810208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -22920,6 +24122,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -23951,6 +25233,998 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -24104,8 +26378,159 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14969</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>83003</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>672799</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>74195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="תמונה 1" descr="C:\WINDOWS\system32\cmd.exe"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="21016"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6083755" y="6260646"/>
+          <a:ext cx="4856389" cy="5134692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127908</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>14968</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>730251</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>6160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="תמונה 2" descr="C:\WINDOWS\system32\cmd.exe"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect r="24318"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127908" y="6192611"/>
+          <a:ext cx="4648200" cy="5134692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>172809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1646465</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>58509</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="תרשים 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>20411</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>186417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>72117</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="תרשים 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:C19" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:C19" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A12:C19"/>
   <tableColumns count="3">
     <tableColumn id="1" name="alpha"/>
@@ -24116,8 +26541,34 @@
 </table>
 </file>
 
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="טבלה2" displayName="טבלה2" ref="M3:P8" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="M3:P8"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="alpha" dataDxfId="9"/>
+    <tableColumn id="2" name="iterations" dataDxfId="8"/>
+    <tableColumn id="3" name="prediction on test data" dataDxfId="7"/>
+    <tableColumn id="4" name="prediction on training data" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="טבלה24" displayName="טבלה24" ref="M25:P30" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="M25:P30"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="alpha" dataDxfId="3"/>
+    <tableColumn id="2" name="iterations" dataDxfId="0"/>
+    <tableColumn id="3" name="prediction on test data" dataDxfId="2"/>
+    <tableColumn id="4" name="prediction on training data" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -24381,8 +26832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:SF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36512,4 +38963,968 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R39" sqref="R39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.92936799999999997</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.78333299999999995</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.93308599999999997</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.78333299999999995</v>
+      </c>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.68029700000000004</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.78333299999999995</v>
+      </c>
+      <c r="E4" s="3">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.67657999999999996</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.78333299999999995</v>
+      </c>
+      <c r="K4" s="3">
+        <v>15</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N4" s="3">
+        <f>$B$2</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
+        <f>C$7</f>
+        <v>0.39405200000000001</v>
+      </c>
+      <c r="P4" s="3">
+        <f>D$7</f>
+        <v>0.60333300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.70631999999999995</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.79666700000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.70260199999999995</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.78</v>
+      </c>
+      <c r="K5" s="3">
+        <v>10</v>
+      </c>
+      <c r="M5" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="3">
+        <f>$B$8</f>
+        <v>51</v>
+      </c>
+      <c r="O5" s="3">
+        <f>C$13</f>
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="P5" s="3">
+        <f>D$13</f>
+        <v>0.906667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.66171000000000002</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.77333300000000005</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.44981399999999999</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="K6" s="3">
+        <v>19</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="3">
+        <f>$B$14</f>
+        <v>101</v>
+      </c>
+      <c r="O6" s="3">
+        <f>C19</f>
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="P6" s="3">
+        <f>D19</f>
+        <v>0.93333299999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.39405200000000001</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.60333300000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.44609700000000002</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.62333300000000003</v>
+      </c>
+      <c r="K7" s="3">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N7" s="3">
+        <f>$B$20</f>
+        <v>151</v>
+      </c>
+      <c r="O7" s="3">
+        <f>C25</f>
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="P7" s="3">
+        <f>D25</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>51</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="N8" s="3">
+        <f>$B$26</f>
+        <v>201</v>
+      </c>
+      <c r="O8" s="3">
+        <f>C31</f>
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="P8" s="3">
+        <f>D31</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="E9" s="3">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.843333</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.86333300000000002</v>
+      </c>
+      <c r="E10" s="3">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="K10" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.89333300000000004</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.93333299999999997</v>
+      </c>
+      <c r="K11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.88666699999999998</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="K12" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.906667</v>
+      </c>
+      <c r="E13" s="3">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.94052000000000002</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="K13" s="3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.84666699999999995</v>
+      </c>
+      <c r="E15" s="3">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.86666699999999997</v>
+      </c>
+      <c r="K15" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.96282500000000004</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K16" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.95910799999999996</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.93333299999999997</v>
+      </c>
+      <c r="E17" s="3">
+        <v>25</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K17" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.95538999999999996</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.906667</v>
+      </c>
+      <c r="E18" s="3">
+        <v>8</v>
+      </c>
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.94333299999999998</v>
+      </c>
+      <c r="K18" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.93333299999999997</v>
+      </c>
+      <c r="E19" s="3">
+        <v>28</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>151</v>
+      </c>
+      <c r="G20" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.86666699999999997</v>
+      </c>
+      <c r="E21" s="3">
+        <v>24</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K21" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.96282500000000004</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.96282500000000004</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="K22" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E23" s="3">
+        <v>8</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.95538999999999996</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K23" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.94333299999999998</v>
+      </c>
+      <c r="E24" s="3">
+        <v>22</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K24" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K25" s="3">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" t="s">
+        <v>4</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>201</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>201</v>
+      </c>
+      <c r="M26" s="3">
+        <v>2</v>
+      </c>
+      <c r="N26" s="3">
+        <f>$B$2</f>
+        <v>1</v>
+      </c>
+      <c r="O26" s="3">
+        <f>I7</f>
+        <v>0.44609700000000002</v>
+      </c>
+      <c r="P26" s="3">
+        <f>J7</f>
+        <v>0.62333300000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="E27" s="3">
+        <v>24</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.94795499999999999</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K27" s="3">
+        <v>24</v>
+      </c>
+      <c r="M27" s="3">
+        <v>2</v>
+      </c>
+      <c r="N27" s="3">
+        <f>$B$8</f>
+        <v>51</v>
+      </c>
+      <c r="O27" s="3">
+        <f>I13</f>
+        <v>0.94052000000000002</v>
+      </c>
+      <c r="P27" s="3">
+        <f>J13</f>
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.96282500000000004</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.91333299999999995</v>
+      </c>
+      <c r="E28" s="3">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.95910799999999996</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.96333299999999999</v>
+      </c>
+      <c r="K28" s="3">
+        <v>25</v>
+      </c>
+      <c r="M28" s="3">
+        <v>2</v>
+      </c>
+      <c r="N28" s="3">
+        <f>$B$14</f>
+        <v>101</v>
+      </c>
+      <c r="O28" s="3">
+        <f>I19</f>
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="P28" s="3">
+        <f>J19</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.95538999999999996</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E29" s="3">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.97026000000000001</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.96</v>
+      </c>
+      <c r="K29" s="3">
+        <v>8</v>
+      </c>
+      <c r="M29" s="3">
+        <v>2</v>
+      </c>
+      <c r="N29" s="3">
+        <f>$B$20</f>
+        <v>151</v>
+      </c>
+      <c r="O29" s="3">
+        <f>I25</f>
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="P29" s="3">
+        <f>J25</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.95167299999999999</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E30" s="3">
+        <v>22</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.97397800000000001</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.95666700000000005</v>
+      </c>
+      <c r="K30" s="3">
+        <v>12</v>
+      </c>
+      <c r="M30" s="3">
+        <v>2</v>
+      </c>
+      <c r="N30" s="3">
+        <f>$B$26</f>
+        <v>201</v>
+      </c>
+      <c r="O30" s="3">
+        <f>I31</f>
+        <v>0.97397800000000001</v>
+      </c>
+      <c r="P30" s="3">
+        <f>J31</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.94423800000000002</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.97397800000000001</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K31" s="3">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>